<commit_message>
Adding employment and school data
</commit_message>
<xml_diff>
--- a/output/TAZ1454 2015 Land Use.xlsx
+++ b/output/TAZ1454 2015 Land Use.xlsx
@@ -13,6 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Data Sources" sheetId="1" r:id="rId1"/>
+    <sheet name="2010 District Summary" sheetId="2" r:id="rId2"/>
+    <sheet name="2015 District Summary" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="102">
   <si>
     <t>ZONE</t>
   </si>
@@ -327,6 +329,9 @@
   </si>
   <si>
     <t>B09019</t>
+  </si>
+  <si>
+    <t>2040 PBA, 2015 Model Run</t>
   </si>
 </sst>
 </file>
@@ -681,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="48.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1146,7 +1151,7 @@
         <v>79</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D37" s="1"/>
     </row>
@@ -1158,7 +1163,7 @@
         <v>80</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D38" s="1"/>
     </row>
@@ -1170,7 +1175,7 @@
         <v>81</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D39" s="1"/>
     </row>
@@ -1254,4 +1259,2623 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>79818</v>
+      </c>
+      <c r="C2">
+        <v>139465</v>
+      </c>
+      <c r="D2">
+        <v>147425</v>
+      </c>
+      <c r="E2">
+        <v>74265</v>
+      </c>
+      <c r="F2">
+        <v>1735</v>
+      </c>
+      <c r="G2">
+        <v>88597</v>
+      </c>
+      <c r="H2">
+        <v>33907</v>
+      </c>
+      <c r="I2">
+        <v>20722</v>
+      </c>
+      <c r="J2">
+        <v>12679</v>
+      </c>
+      <c r="K2">
+        <v>12510</v>
+      </c>
+      <c r="L2">
+        <v>348046</v>
+      </c>
+      <c r="M2">
+        <v>4472</v>
+      </c>
+      <c r="N2">
+        <v>10818</v>
+      </c>
+      <c r="O2">
+        <v>66600</v>
+      </c>
+      <c r="P2">
+        <v>42059</v>
+      </c>
+      <c r="Q2">
+        <v>23476</v>
+      </c>
+      <c r="R2">
+        <v>19465</v>
+      </c>
+      <c r="S2">
+        <v>154411</v>
+      </c>
+      <c r="T2">
+        <v>86226</v>
+      </c>
+      <c r="U2">
+        <v>69940</v>
+      </c>
+      <c r="V2">
+        <v>401</v>
+      </c>
+      <c r="W2">
+        <v>17603</v>
+      </c>
+      <c r="X2">
+        <v>7960</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>106321</v>
+      </c>
+      <c r="C3">
+        <v>210475</v>
+      </c>
+      <c r="D3">
+        <v>216130</v>
+      </c>
+      <c r="E3">
+        <v>124607</v>
+      </c>
+      <c r="F3">
+        <v>16917</v>
+      </c>
+      <c r="G3">
+        <v>94806</v>
+      </c>
+      <c r="H3">
+        <v>28331</v>
+      </c>
+      <c r="I3">
+        <v>28018</v>
+      </c>
+      <c r="J3">
+        <v>21717</v>
+      </c>
+      <c r="K3">
+        <v>28255</v>
+      </c>
+      <c r="L3">
+        <v>84789</v>
+      </c>
+      <c r="M3">
+        <v>8560</v>
+      </c>
+      <c r="N3">
+        <v>18573</v>
+      </c>
+      <c r="O3">
+        <v>104536</v>
+      </c>
+      <c r="P3">
+        <v>55283</v>
+      </c>
+      <c r="Q3">
+        <v>29178</v>
+      </c>
+      <c r="R3">
+        <v>8177</v>
+      </c>
+      <c r="S3">
+        <v>12053</v>
+      </c>
+      <c r="T3">
+        <v>38186</v>
+      </c>
+      <c r="U3">
+        <v>23549</v>
+      </c>
+      <c r="V3">
+        <v>103</v>
+      </c>
+      <c r="W3">
+        <v>2721</v>
+      </c>
+      <c r="X3">
+        <v>5655</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>122685</v>
+      </c>
+      <c r="C4">
+        <v>329797</v>
+      </c>
+      <c r="D4">
+        <v>336452</v>
+      </c>
+      <c r="E4">
+        <v>167164</v>
+      </c>
+      <c r="F4">
+        <v>60176</v>
+      </c>
+      <c r="G4">
+        <v>70891</v>
+      </c>
+      <c r="H4">
+        <v>36682</v>
+      </c>
+      <c r="I4">
+        <v>32905</v>
+      </c>
+      <c r="J4">
+        <v>26007</v>
+      </c>
+      <c r="K4">
+        <v>27091</v>
+      </c>
+      <c r="L4">
+        <v>152075</v>
+      </c>
+      <c r="M4">
+        <v>20919</v>
+      </c>
+      <c r="N4">
+        <v>50383</v>
+      </c>
+      <c r="O4">
+        <v>136419</v>
+      </c>
+      <c r="P4">
+        <v>90421</v>
+      </c>
+      <c r="Q4">
+        <v>38310</v>
+      </c>
+      <c r="R4">
+        <v>10950</v>
+      </c>
+      <c r="S4">
+        <v>29750</v>
+      </c>
+      <c r="T4">
+        <v>61422</v>
+      </c>
+      <c r="U4">
+        <v>35961</v>
+      </c>
+      <c r="V4">
+        <v>138</v>
+      </c>
+      <c r="W4">
+        <v>13854</v>
+      </c>
+      <c r="X4">
+        <v>6655</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>49104</v>
+      </c>
+      <c r="C5">
+        <v>131276</v>
+      </c>
+      <c r="D5">
+        <v>134052</v>
+      </c>
+      <c r="E5">
+        <v>63773</v>
+      </c>
+      <c r="F5">
+        <v>35338</v>
+      </c>
+      <c r="G5">
+        <v>16874</v>
+      </c>
+      <c r="H5">
+        <v>11686</v>
+      </c>
+      <c r="I5">
+        <v>13350</v>
+      </c>
+      <c r="J5">
+        <v>11265</v>
+      </c>
+      <c r="K5">
+        <v>12803</v>
+      </c>
+      <c r="L5">
+        <v>27600</v>
+      </c>
+      <c r="M5">
+        <v>6650</v>
+      </c>
+      <c r="N5">
+        <v>18698</v>
+      </c>
+      <c r="O5">
+        <v>48168</v>
+      </c>
+      <c r="P5">
+        <v>38735</v>
+      </c>
+      <c r="Q5">
+        <v>21801</v>
+      </c>
+      <c r="R5">
+        <v>5389</v>
+      </c>
+      <c r="S5">
+        <v>4547</v>
+      </c>
+      <c r="T5">
+        <v>10422</v>
+      </c>
+      <c r="U5">
+        <v>6313</v>
+      </c>
+      <c r="V5">
+        <v>13</v>
+      </c>
+      <c r="W5">
+        <v>916</v>
+      </c>
+      <c r="X5">
+        <v>2776</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>96515</v>
+      </c>
+      <c r="C6">
+        <v>284409</v>
+      </c>
+      <c r="D6">
+        <v>287104</v>
+      </c>
+      <c r="E6">
+        <v>133950</v>
+      </c>
+      <c r="F6">
+        <v>72233</v>
+      </c>
+      <c r="G6">
+        <v>31477</v>
+      </c>
+      <c r="H6">
+        <v>19400</v>
+      </c>
+      <c r="I6">
+        <v>25349</v>
+      </c>
+      <c r="J6">
+        <v>26028</v>
+      </c>
+      <c r="K6">
+        <v>25738</v>
+      </c>
+      <c r="L6">
+        <v>108571</v>
+      </c>
+      <c r="M6">
+        <v>15763</v>
+      </c>
+      <c r="N6">
+        <v>54148</v>
+      </c>
+      <c r="O6">
+        <v>98103</v>
+      </c>
+      <c r="P6">
+        <v>80881</v>
+      </c>
+      <c r="Q6">
+        <v>38209</v>
+      </c>
+      <c r="R6">
+        <v>14394</v>
+      </c>
+      <c r="S6">
+        <v>20160</v>
+      </c>
+      <c r="T6">
+        <v>31616</v>
+      </c>
+      <c r="U6">
+        <v>16241</v>
+      </c>
+      <c r="V6">
+        <v>376</v>
+      </c>
+      <c r="W6">
+        <v>25784</v>
+      </c>
+      <c r="X6">
+        <v>2695</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>83567</v>
+      </c>
+      <c r="C7">
+        <v>210973</v>
+      </c>
+      <c r="D7">
+        <v>213427</v>
+      </c>
+      <c r="E7">
+        <v>102758</v>
+      </c>
+      <c r="F7">
+        <v>56264</v>
+      </c>
+      <c r="G7">
+        <v>32621</v>
+      </c>
+      <c r="H7">
+        <v>14813</v>
+      </c>
+      <c r="I7">
+        <v>18848</v>
+      </c>
+      <c r="J7">
+        <v>19710</v>
+      </c>
+      <c r="K7">
+        <v>30196</v>
+      </c>
+      <c r="L7">
+        <v>100175</v>
+      </c>
+      <c r="M7">
+        <v>11718</v>
+      </c>
+      <c r="N7">
+        <v>35024</v>
+      </c>
+      <c r="O7">
+        <v>73472</v>
+      </c>
+      <c r="P7">
+        <v>63451</v>
+      </c>
+      <c r="Q7">
+        <v>29762</v>
+      </c>
+      <c r="R7">
+        <v>11502</v>
+      </c>
+      <c r="S7">
+        <v>35889</v>
+      </c>
+      <c r="T7">
+        <v>27044</v>
+      </c>
+      <c r="U7">
+        <v>14858</v>
+      </c>
+      <c r="V7">
+        <v>730</v>
+      </c>
+      <c r="W7">
+        <v>10152</v>
+      </c>
+      <c r="X7">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>77936</v>
+      </c>
+      <c r="C8">
+        <v>218313</v>
+      </c>
+      <c r="D8">
+        <v>221210</v>
+      </c>
+      <c r="E8">
+        <v>98632</v>
+      </c>
+      <c r="F8">
+        <v>58679</v>
+      </c>
+      <c r="G8">
+        <v>23937</v>
+      </c>
+      <c r="H8">
+        <v>13827</v>
+      </c>
+      <c r="I8">
+        <v>17087</v>
+      </c>
+      <c r="J8">
+        <v>17114</v>
+      </c>
+      <c r="K8">
+        <v>29908</v>
+      </c>
+      <c r="L8">
+        <v>129842</v>
+      </c>
+      <c r="M8">
+        <v>15432</v>
+      </c>
+      <c r="N8">
+        <v>42905</v>
+      </c>
+      <c r="O8">
+        <v>77724</v>
+      </c>
+      <c r="P8">
+        <v>58736</v>
+      </c>
+      <c r="Q8">
+        <v>26413</v>
+      </c>
+      <c r="R8">
+        <v>8970</v>
+      </c>
+      <c r="S8">
+        <v>35784</v>
+      </c>
+      <c r="T8">
+        <v>29007</v>
+      </c>
+      <c r="U8">
+        <v>29017</v>
+      </c>
+      <c r="V8">
+        <v>1428</v>
+      </c>
+      <c r="W8">
+        <v>25636</v>
+      </c>
+      <c r="X8">
+        <v>2897</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>71929</v>
+      </c>
+      <c r="C9">
+        <v>175214</v>
+      </c>
+      <c r="D9">
+        <v>182560</v>
+      </c>
+      <c r="E9">
+        <v>85887</v>
+      </c>
+      <c r="F9">
+        <v>44384</v>
+      </c>
+      <c r="G9">
+        <v>32215</v>
+      </c>
+      <c r="H9">
+        <v>17817</v>
+      </c>
+      <c r="I9">
+        <v>16029</v>
+      </c>
+      <c r="J9">
+        <v>14528</v>
+      </c>
+      <c r="K9">
+        <v>23555</v>
+      </c>
+      <c r="L9">
+        <v>157160</v>
+      </c>
+      <c r="M9">
+        <v>8913</v>
+      </c>
+      <c r="N9">
+        <v>30004</v>
+      </c>
+      <c r="O9">
+        <v>62443</v>
+      </c>
+      <c r="P9">
+        <v>52536</v>
+      </c>
+      <c r="Q9">
+        <v>28664</v>
+      </c>
+      <c r="R9">
+        <v>9959</v>
+      </c>
+      <c r="S9">
+        <v>39339</v>
+      </c>
+      <c r="T9">
+        <v>75927</v>
+      </c>
+      <c r="U9">
+        <v>18368</v>
+      </c>
+      <c r="V9">
+        <v>171</v>
+      </c>
+      <c r="W9">
+        <v>13396</v>
+      </c>
+      <c r="X9">
+        <v>7346</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>107259</v>
+      </c>
+      <c r="C10">
+        <v>272629</v>
+      </c>
+      <c r="D10">
+        <v>274049</v>
+      </c>
+      <c r="E10">
+        <v>131985</v>
+      </c>
+      <c r="F10">
+        <v>45307</v>
+      </c>
+      <c r="G10">
+        <v>70669</v>
+      </c>
+      <c r="H10">
+        <v>35473</v>
+      </c>
+      <c r="I10">
+        <v>24275</v>
+      </c>
+      <c r="J10">
+        <v>23936</v>
+      </c>
+      <c r="K10">
+        <v>23575</v>
+      </c>
+      <c r="L10">
+        <v>285978</v>
+      </c>
+      <c r="M10">
+        <v>18322</v>
+      </c>
+      <c r="N10">
+        <v>41149</v>
+      </c>
+      <c r="O10">
+        <v>117367</v>
+      </c>
+      <c r="P10">
+        <v>67794</v>
+      </c>
+      <c r="Q10">
+        <v>29417</v>
+      </c>
+      <c r="R10">
+        <v>13786</v>
+      </c>
+      <c r="S10">
+        <v>72588</v>
+      </c>
+      <c r="T10">
+        <v>37253</v>
+      </c>
+      <c r="U10">
+        <v>50793</v>
+      </c>
+      <c r="V10">
+        <v>735</v>
+      </c>
+      <c r="W10">
+        <v>110823</v>
+      </c>
+      <c r="X10">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>116656</v>
+      </c>
+      <c r="C11">
+        <v>312555</v>
+      </c>
+      <c r="D11">
+        <v>314805</v>
+      </c>
+      <c r="E11">
+        <v>139878</v>
+      </c>
+      <c r="F11">
+        <v>86003</v>
+      </c>
+      <c r="G11">
+        <v>40791</v>
+      </c>
+      <c r="H11">
+        <v>26211</v>
+      </c>
+      <c r="I11">
+        <v>27081</v>
+      </c>
+      <c r="J11">
+        <v>26711</v>
+      </c>
+      <c r="K11">
+        <v>36653</v>
+      </c>
+      <c r="L11">
+        <v>119715</v>
+      </c>
+      <c r="M11">
+        <v>18644</v>
+      </c>
+      <c r="N11">
+        <v>60956</v>
+      </c>
+      <c r="O11">
+        <v>102155</v>
+      </c>
+      <c r="P11">
+        <v>91320</v>
+      </c>
+      <c r="Q11">
+        <v>41730</v>
+      </c>
+      <c r="R11">
+        <v>17229</v>
+      </c>
+      <c r="S11">
+        <v>25176</v>
+      </c>
+      <c r="T11">
+        <v>37749</v>
+      </c>
+      <c r="U11">
+        <v>22384</v>
+      </c>
+      <c r="V11">
+        <v>292</v>
+      </c>
+      <c r="W11">
+        <v>16885</v>
+      </c>
+      <c r="X11">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>107048</v>
+      </c>
+      <c r="C12">
+        <v>302498</v>
+      </c>
+      <c r="D12">
+        <v>312896</v>
+      </c>
+      <c r="E12">
+        <v>135083</v>
+      </c>
+      <c r="F12">
+        <v>58687</v>
+      </c>
+      <c r="G12">
+        <v>58329</v>
+      </c>
+      <c r="H12">
+        <v>40677</v>
+      </c>
+      <c r="I12">
+        <v>27776</v>
+      </c>
+      <c r="J12">
+        <v>21478</v>
+      </c>
+      <c r="K12">
+        <v>17117</v>
+      </c>
+      <c r="L12">
+        <v>135747</v>
+      </c>
+      <c r="M12">
+        <v>21863</v>
+      </c>
+      <c r="N12">
+        <v>64471</v>
+      </c>
+      <c r="O12">
+        <v>119919</v>
+      </c>
+      <c r="P12">
+        <v>72106</v>
+      </c>
+      <c r="Q12">
+        <v>34537</v>
+      </c>
+      <c r="R12">
+        <v>10230</v>
+      </c>
+      <c r="S12">
+        <v>33569</v>
+      </c>
+      <c r="T12">
+        <v>32852</v>
+      </c>
+      <c r="U12">
+        <v>42010</v>
+      </c>
+      <c r="V12">
+        <v>370</v>
+      </c>
+      <c r="W12">
+        <v>16716</v>
+      </c>
+      <c r="X12">
+        <v>10398</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>107579</v>
+      </c>
+      <c r="C13">
+        <v>394077</v>
+      </c>
+      <c r="D13">
+        <v>397077</v>
+      </c>
+      <c r="E13">
+        <v>164740</v>
+      </c>
+      <c r="F13">
+        <v>87606</v>
+      </c>
+      <c r="G13">
+        <v>27935</v>
+      </c>
+      <c r="H13">
+        <v>28436</v>
+      </c>
+      <c r="I13">
+        <v>24987</v>
+      </c>
+      <c r="J13">
+        <v>26479</v>
+      </c>
+      <c r="K13">
+        <v>27677</v>
+      </c>
+      <c r="L13">
+        <v>107978</v>
+      </c>
+      <c r="M13">
+        <v>29116</v>
+      </c>
+      <c r="N13">
+        <v>90333</v>
+      </c>
+      <c r="O13">
+        <v>140498</v>
+      </c>
+      <c r="P13">
+        <v>101591</v>
+      </c>
+      <c r="Q13">
+        <v>35539</v>
+      </c>
+      <c r="R13">
+        <v>13116</v>
+      </c>
+      <c r="S13">
+        <v>18582</v>
+      </c>
+      <c r="T13">
+        <v>26410</v>
+      </c>
+      <c r="U13">
+        <v>25119</v>
+      </c>
+      <c r="V13">
+        <v>287</v>
+      </c>
+      <c r="W13">
+        <v>24464</v>
+      </c>
+      <c r="X13">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>70615</v>
+      </c>
+      <c r="C14">
+        <v>213771</v>
+      </c>
+      <c r="D14">
+        <v>214724</v>
+      </c>
+      <c r="E14">
+        <v>98525</v>
+      </c>
+      <c r="F14">
+        <v>58589</v>
+      </c>
+      <c r="G14">
+        <v>17619</v>
+      </c>
+      <c r="H14">
+        <v>15025</v>
+      </c>
+      <c r="I14">
+        <v>15987</v>
+      </c>
+      <c r="J14">
+        <v>18137</v>
+      </c>
+      <c r="K14">
+        <v>21466</v>
+      </c>
+      <c r="L14">
+        <v>52350</v>
+      </c>
+      <c r="M14">
+        <v>14706</v>
+      </c>
+      <c r="N14">
+        <v>47191</v>
+      </c>
+      <c r="O14">
+        <v>71438</v>
+      </c>
+      <c r="P14">
+        <v>63377</v>
+      </c>
+      <c r="Q14">
+        <v>18012</v>
+      </c>
+      <c r="R14">
+        <v>8798</v>
+      </c>
+      <c r="S14">
+        <v>11986</v>
+      </c>
+      <c r="T14">
+        <v>14816</v>
+      </c>
+      <c r="U14">
+        <v>8612</v>
+      </c>
+      <c r="V14">
+        <v>319</v>
+      </c>
+      <c r="W14">
+        <v>7819</v>
+      </c>
+      <c r="X14">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>31407</v>
+      </c>
+      <c r="C15">
+        <v>101717</v>
+      </c>
+      <c r="D15">
+        <v>103171</v>
+      </c>
+      <c r="E15">
+        <v>43098</v>
+      </c>
+      <c r="F15">
+        <v>27707</v>
+      </c>
+      <c r="G15">
+        <v>8416</v>
+      </c>
+      <c r="H15">
+        <v>7943</v>
+      </c>
+      <c r="I15">
+        <v>7509</v>
+      </c>
+      <c r="J15">
+        <v>7618</v>
+      </c>
+      <c r="K15">
+        <v>8337</v>
+      </c>
+      <c r="L15">
+        <v>44408</v>
+      </c>
+      <c r="M15">
+        <v>7853</v>
+      </c>
+      <c r="N15">
+        <v>26104</v>
+      </c>
+      <c r="O15">
+        <v>31880</v>
+      </c>
+      <c r="P15">
+        <v>28557</v>
+      </c>
+      <c r="Q15">
+        <v>8777</v>
+      </c>
+      <c r="R15">
+        <v>6388</v>
+      </c>
+      <c r="S15">
+        <v>7268</v>
+      </c>
+      <c r="T15">
+        <v>10588</v>
+      </c>
+      <c r="U15">
+        <v>7936</v>
+      </c>
+      <c r="V15">
+        <v>2900</v>
+      </c>
+      <c r="W15">
+        <v>9328</v>
+      </c>
+      <c r="X15">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>71358</v>
+      </c>
+      <c r="C16">
+        <v>197468</v>
+      </c>
+      <c r="D16">
+        <v>199235</v>
+      </c>
+      <c r="E16">
+        <v>97318</v>
+      </c>
+      <c r="F16">
+        <v>56091</v>
+      </c>
+      <c r="G16">
+        <v>17007</v>
+      </c>
+      <c r="H16">
+        <v>14658</v>
+      </c>
+      <c r="I16">
+        <v>15195</v>
+      </c>
+      <c r="J16">
+        <v>18438</v>
+      </c>
+      <c r="K16">
+        <v>23067</v>
+      </c>
+      <c r="L16">
+        <v>121963</v>
+      </c>
+      <c r="M16">
+        <v>13848</v>
+      </c>
+      <c r="N16">
+        <v>39368</v>
+      </c>
+      <c r="O16">
+        <v>76840</v>
+      </c>
+      <c r="P16">
+        <v>54258</v>
+      </c>
+      <c r="Q16">
+        <v>14921</v>
+      </c>
+      <c r="R16">
+        <v>18406</v>
+      </c>
+      <c r="S16">
+        <v>34252</v>
+      </c>
+      <c r="T16">
+        <v>22155</v>
+      </c>
+      <c r="U16">
+        <v>30144</v>
+      </c>
+      <c r="V16">
+        <v>525</v>
+      </c>
+      <c r="W16">
+        <v>16481</v>
+      </c>
+      <c r="X16">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>103634</v>
+      </c>
+      <c r="C17">
+        <v>322812</v>
+      </c>
+      <c r="D17">
+        <v>325130</v>
+      </c>
+      <c r="E17">
+        <v>161703</v>
+      </c>
+      <c r="F17">
+        <v>73777</v>
+      </c>
+      <c r="G17">
+        <v>29246</v>
+      </c>
+      <c r="H17">
+        <v>21207</v>
+      </c>
+      <c r="I17">
+        <v>25850</v>
+      </c>
+      <c r="J17">
+        <v>27872</v>
+      </c>
+      <c r="K17">
+        <v>28705</v>
+      </c>
+      <c r="L17">
+        <v>119762</v>
+      </c>
+      <c r="M17">
+        <v>24036</v>
+      </c>
+      <c r="N17">
+        <v>63759</v>
+      </c>
+      <c r="O17">
+        <v>127668</v>
+      </c>
+      <c r="P17">
+        <v>81570</v>
+      </c>
+      <c r="Q17">
+        <v>28097</v>
+      </c>
+      <c r="R17">
+        <v>12821</v>
+      </c>
+      <c r="S17">
+        <v>24598</v>
+      </c>
+      <c r="T17">
+        <v>27783</v>
+      </c>
+      <c r="U17">
+        <v>19185</v>
+      </c>
+      <c r="V17">
+        <v>199</v>
+      </c>
+      <c r="W17">
+        <v>35176</v>
+      </c>
+      <c r="X17">
+        <v>2318</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>121755</v>
+      </c>
+      <c r="C18">
+        <v>359395</v>
+      </c>
+      <c r="D18">
+        <v>365034</v>
+      </c>
+      <c r="E18">
+        <v>169109</v>
+      </c>
+      <c r="F18">
+        <v>85879</v>
+      </c>
+      <c r="G18">
+        <v>39520</v>
+      </c>
+      <c r="H18">
+        <v>35077</v>
+      </c>
+      <c r="I18">
+        <v>39001</v>
+      </c>
+      <c r="J18">
+        <v>28509</v>
+      </c>
+      <c r="K18">
+        <v>19168</v>
+      </c>
+      <c r="L18">
+        <v>127113</v>
+      </c>
+      <c r="M18">
+        <v>25929</v>
+      </c>
+      <c r="N18">
+        <v>69001</v>
+      </c>
+      <c r="O18">
+        <v>133410</v>
+      </c>
+      <c r="P18">
+        <v>89150</v>
+      </c>
+      <c r="Q18">
+        <v>47544</v>
+      </c>
+      <c r="R18">
+        <v>13491</v>
+      </c>
+      <c r="S18">
+        <v>17455</v>
+      </c>
+      <c r="T18">
+        <v>31308</v>
+      </c>
+      <c r="U18">
+        <v>28313</v>
+      </c>
+      <c r="V18">
+        <v>121</v>
+      </c>
+      <c r="W18">
+        <v>36425</v>
+      </c>
+      <c r="X18">
+        <v>5639</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>180845</v>
+      </c>
+      <c r="C19">
+        <v>457333</v>
+      </c>
+      <c r="D19">
+        <v>465535</v>
+      </c>
+      <c r="E19">
+        <v>214784</v>
+      </c>
+      <c r="F19">
+        <v>96275</v>
+      </c>
+      <c r="G19">
+        <v>88871</v>
+      </c>
+      <c r="H19">
+        <v>69207</v>
+      </c>
+      <c r="I19">
+        <v>53287</v>
+      </c>
+      <c r="J19">
+        <v>31957</v>
+      </c>
+      <c r="K19">
+        <v>26394</v>
+      </c>
+      <c r="L19">
+        <v>207226</v>
+      </c>
+      <c r="M19">
+        <v>32181</v>
+      </c>
+      <c r="N19">
+        <v>87939</v>
+      </c>
+      <c r="O19">
+        <v>174388</v>
+      </c>
+      <c r="P19">
+        <v>117784</v>
+      </c>
+      <c r="Q19">
+        <v>53243</v>
+      </c>
+      <c r="R19">
+        <v>11588</v>
+      </c>
+      <c r="S19">
+        <v>39230</v>
+      </c>
+      <c r="T19">
+        <v>65517</v>
+      </c>
+      <c r="U19">
+        <v>68145</v>
+      </c>
+      <c r="V19">
+        <v>306</v>
+      </c>
+      <c r="W19">
+        <v>22440</v>
+      </c>
+      <c r="X19">
+        <v>8202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>73989</v>
+      </c>
+      <c r="C20">
+        <v>161035</v>
+      </c>
+      <c r="D20">
+        <v>174639</v>
+      </c>
+      <c r="E20">
+        <v>89737</v>
+      </c>
+      <c r="F20">
+        <v>36961</v>
+      </c>
+      <c r="G20">
+        <v>38020</v>
+      </c>
+      <c r="H20">
+        <v>27208</v>
+      </c>
+      <c r="I20">
+        <v>20787</v>
+      </c>
+      <c r="J20">
+        <v>13176</v>
+      </c>
+      <c r="K20">
+        <v>12818</v>
+      </c>
+      <c r="L20">
+        <v>127523</v>
+      </c>
+      <c r="M20">
+        <v>7352</v>
+      </c>
+      <c r="N20">
+        <v>24916</v>
+      </c>
+      <c r="O20">
+        <v>79495</v>
+      </c>
+      <c r="P20">
+        <v>44580</v>
+      </c>
+      <c r="Q20">
+        <v>18296</v>
+      </c>
+      <c r="R20">
+        <v>8462</v>
+      </c>
+      <c r="S20">
+        <v>33319</v>
+      </c>
+      <c r="T20">
+        <v>51581</v>
+      </c>
+      <c r="U20">
+        <v>22844</v>
+      </c>
+      <c r="V20">
+        <v>66</v>
+      </c>
+      <c r="W20">
+        <v>11251</v>
+      </c>
+      <c r="X20">
+        <v>13604</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>89624</v>
+      </c>
+      <c r="C21">
+        <v>253924</v>
+      </c>
+      <c r="D21">
+        <v>255574</v>
+      </c>
+      <c r="E21">
+        <v>116416</v>
+      </c>
+      <c r="F21">
+        <v>66717</v>
+      </c>
+      <c r="G21">
+        <v>28956</v>
+      </c>
+      <c r="H21">
+        <v>28465</v>
+      </c>
+      <c r="I21">
+        <v>27659</v>
+      </c>
+      <c r="J21">
+        <v>19768</v>
+      </c>
+      <c r="K21">
+        <v>13732</v>
+      </c>
+      <c r="L21">
+        <v>61490</v>
+      </c>
+      <c r="M21">
+        <v>16626</v>
+      </c>
+      <c r="N21">
+        <v>50681</v>
+      </c>
+      <c r="O21">
+        <v>89346</v>
+      </c>
+      <c r="P21">
+        <v>66233</v>
+      </c>
+      <c r="Q21">
+        <v>32688</v>
+      </c>
+      <c r="R21">
+        <v>8209</v>
+      </c>
+      <c r="S21">
+        <v>10219</v>
+      </c>
+      <c r="T21">
+        <v>17602</v>
+      </c>
+      <c r="U21">
+        <v>13387</v>
+      </c>
+      <c r="V21">
+        <v>255</v>
+      </c>
+      <c r="W21">
+        <v>11818</v>
+      </c>
+      <c r="X21">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>82688</v>
+      </c>
+      <c r="C22">
+        <v>217383</v>
+      </c>
+      <c r="D22">
+        <v>219644</v>
+      </c>
+      <c r="E22">
+        <v>113956</v>
+      </c>
+      <c r="F22">
+        <v>63830</v>
+      </c>
+      <c r="G22">
+        <v>26800</v>
+      </c>
+      <c r="H22">
+        <v>19723</v>
+      </c>
+      <c r="I22">
+        <v>23642</v>
+      </c>
+      <c r="J22">
+        <v>21107</v>
+      </c>
+      <c r="K22">
+        <v>18216</v>
+      </c>
+      <c r="L22">
+        <v>101115</v>
+      </c>
+      <c r="M22">
+        <v>13521</v>
+      </c>
+      <c r="N22">
+        <v>39445</v>
+      </c>
+      <c r="O22">
+        <v>79423</v>
+      </c>
+      <c r="P22">
+        <v>60137</v>
+      </c>
+      <c r="Q22">
+        <v>27118</v>
+      </c>
+      <c r="R22">
+        <v>10276</v>
+      </c>
+      <c r="S22">
+        <v>21607</v>
+      </c>
+      <c r="T22">
+        <v>30067</v>
+      </c>
+      <c r="U22">
+        <v>27596</v>
+      </c>
+      <c r="V22">
+        <v>223</v>
+      </c>
+      <c r="W22">
+        <v>11346</v>
+      </c>
+      <c r="X22">
+        <v>2261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>57888</v>
+      </c>
+      <c r="C23">
+        <v>134418</v>
+      </c>
+      <c r="D23">
+        <v>137419</v>
+      </c>
+      <c r="E23">
+        <v>68516</v>
+      </c>
+      <c r="F23">
+        <v>41967</v>
+      </c>
+      <c r="G23">
+        <v>21100</v>
+      </c>
+      <c r="H23">
+        <v>11254</v>
+      </c>
+      <c r="I23">
+        <v>13484</v>
+      </c>
+      <c r="J23">
+        <v>13317</v>
+      </c>
+      <c r="K23">
+        <v>19833</v>
+      </c>
+      <c r="L23">
+        <v>72330</v>
+      </c>
+      <c r="M23">
+        <v>5898</v>
+      </c>
+      <c r="N23">
+        <v>22021</v>
+      </c>
+      <c r="O23">
+        <v>37390</v>
+      </c>
+      <c r="P23">
+        <v>42407</v>
+      </c>
+      <c r="Q23">
+        <v>29703</v>
+      </c>
+      <c r="R23">
+        <v>7330</v>
+      </c>
+      <c r="S23">
+        <v>23516</v>
+      </c>
+      <c r="T23">
+        <v>25658</v>
+      </c>
+      <c r="U23">
+        <v>10773</v>
+      </c>
+      <c r="V23">
+        <v>98</v>
+      </c>
+      <c r="W23">
+        <v>4955</v>
+      </c>
+      <c r="X23">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>51374</v>
+      </c>
+      <c r="C24">
+        <v>145403</v>
+      </c>
+      <c r="D24">
+        <v>145934</v>
+      </c>
+      <c r="E24">
+        <v>73980</v>
+      </c>
+      <c r="F24">
+        <v>48037</v>
+      </c>
+      <c r="G24">
+        <v>6842</v>
+      </c>
+      <c r="H24">
+        <v>5686</v>
+      </c>
+      <c r="I24">
+        <v>8163</v>
+      </c>
+      <c r="J24">
+        <v>11283</v>
+      </c>
+      <c r="K24">
+        <v>26242</v>
+      </c>
+      <c r="L24">
+        <v>69307</v>
+      </c>
+      <c r="M24">
+        <v>9225</v>
+      </c>
+      <c r="N24">
+        <v>29585</v>
+      </c>
+      <c r="O24">
+        <v>44627</v>
+      </c>
+      <c r="P24">
+        <v>49137</v>
+      </c>
+      <c r="Q24">
+        <v>13360</v>
+      </c>
+      <c r="R24">
+        <v>7866</v>
+      </c>
+      <c r="S24">
+        <v>18230</v>
+      </c>
+      <c r="T24">
+        <v>16491</v>
+      </c>
+      <c r="U24">
+        <v>21190</v>
+      </c>
+      <c r="V24">
+        <v>543</v>
+      </c>
+      <c r="W24">
+        <v>4987</v>
+      </c>
+      <c r="X24">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>87034</v>
+      </c>
+      <c r="C25">
+        <v>276289</v>
+      </c>
+      <c r="D25">
+        <v>277811</v>
+      </c>
+      <c r="E25">
+        <v>116252</v>
+      </c>
+      <c r="F25">
+        <v>81388</v>
+      </c>
+      <c r="G25">
+        <v>16670</v>
+      </c>
+      <c r="H25">
+        <v>21976</v>
+      </c>
+      <c r="I25">
+        <v>24600</v>
+      </c>
+      <c r="J25">
+        <v>22911</v>
+      </c>
+      <c r="K25">
+        <v>17547</v>
+      </c>
+      <c r="L25">
+        <v>48106</v>
+      </c>
+      <c r="M25">
+        <v>22210</v>
+      </c>
+      <c r="N25">
+        <v>66113</v>
+      </c>
+      <c r="O25">
+        <v>100354</v>
+      </c>
+      <c r="P25">
+        <v>63674</v>
+      </c>
+      <c r="Q25">
+        <v>25460</v>
+      </c>
+      <c r="R25">
+        <v>8734</v>
+      </c>
+      <c r="S25">
+        <v>8841</v>
+      </c>
+      <c r="T25">
+        <v>16070</v>
+      </c>
+      <c r="U25">
+        <v>10370</v>
+      </c>
+      <c r="V25">
+        <v>340</v>
+      </c>
+      <c r="W25">
+        <v>3751</v>
+      </c>
+      <c r="X25">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>51042</v>
+      </c>
+      <c r="C26">
+        <v>141623</v>
+      </c>
+      <c r="D26">
+        <v>143353</v>
+      </c>
+      <c r="E26">
+        <v>71167</v>
+      </c>
+      <c r="F26">
+        <v>36148</v>
+      </c>
+      <c r="G26">
+        <v>16986</v>
+      </c>
+      <c r="H26">
+        <v>13026</v>
+      </c>
+      <c r="I26">
+        <v>15150</v>
+      </c>
+      <c r="J26">
+        <v>12695</v>
+      </c>
+      <c r="K26">
+        <v>10171</v>
+      </c>
+      <c r="L26">
+        <v>42140</v>
+      </c>
+      <c r="M26">
+        <v>9577</v>
+      </c>
+      <c r="N26">
+        <v>29181</v>
+      </c>
+      <c r="O26">
+        <v>45946</v>
+      </c>
+      <c r="P26">
+        <v>40879</v>
+      </c>
+      <c r="Q26">
+        <v>17770</v>
+      </c>
+      <c r="R26">
+        <v>4849</v>
+      </c>
+      <c r="S26">
+        <v>6354</v>
+      </c>
+      <c r="T26">
+        <v>13487</v>
+      </c>
+      <c r="U26">
+        <v>11204</v>
+      </c>
+      <c r="V26">
+        <v>150</v>
+      </c>
+      <c r="W26">
+        <v>6096</v>
+      </c>
+      <c r="X26">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>85691</v>
+      </c>
+      <c r="C27">
+        <v>247170</v>
+      </c>
+      <c r="D27">
+        <v>257151</v>
+      </c>
+      <c r="E27">
+        <v>120713</v>
+      </c>
+      <c r="F27">
+        <v>73232</v>
+      </c>
+      <c r="G27">
+        <v>16430</v>
+      </c>
+      <c r="H27">
+        <v>21441</v>
+      </c>
+      <c r="I27">
+        <v>24774</v>
+      </c>
+      <c r="J27">
+        <v>23062</v>
+      </c>
+      <c r="K27">
+        <v>16414</v>
+      </c>
+      <c r="L27">
+        <v>79806</v>
+      </c>
+      <c r="M27">
+        <v>18409</v>
+      </c>
+      <c r="N27">
+        <v>54290</v>
+      </c>
+      <c r="O27">
+        <v>91171</v>
+      </c>
+      <c r="P27">
+        <v>66311</v>
+      </c>
+      <c r="Q27">
+        <v>26970</v>
+      </c>
+      <c r="R27">
+        <v>11454</v>
+      </c>
+      <c r="S27">
+        <v>8630</v>
+      </c>
+      <c r="T27">
+        <v>24274</v>
+      </c>
+      <c r="U27">
+        <v>21392</v>
+      </c>
+      <c r="V27">
+        <v>1766</v>
+      </c>
+      <c r="W27">
+        <v>12290</v>
+      </c>
+      <c r="X27">
+        <v>9981</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>33102</v>
+      </c>
+      <c r="C28">
+        <v>94402</v>
+      </c>
+      <c r="D28">
+        <v>95476</v>
+      </c>
+      <c r="E28">
+        <v>44308</v>
+      </c>
+      <c r="F28">
+        <v>28117</v>
+      </c>
+      <c r="G28">
+        <v>9670</v>
+      </c>
+      <c r="H28">
+        <v>9216</v>
+      </c>
+      <c r="I28">
+        <v>9724</v>
+      </c>
+      <c r="J28">
+        <v>8004</v>
+      </c>
+      <c r="K28">
+        <v>6158</v>
+      </c>
+      <c r="L28">
+        <v>43586</v>
+      </c>
+      <c r="M28">
+        <v>6852</v>
+      </c>
+      <c r="N28">
+        <v>20174</v>
+      </c>
+      <c r="O28">
+        <v>31925</v>
+      </c>
+      <c r="P28">
+        <v>23650</v>
+      </c>
+      <c r="Q28">
+        <v>12875</v>
+      </c>
+      <c r="R28">
+        <v>4518</v>
+      </c>
+      <c r="S28">
+        <v>6444</v>
+      </c>
+      <c r="T28">
+        <v>14404</v>
+      </c>
+      <c r="U28">
+        <v>9093</v>
+      </c>
+      <c r="V28">
+        <v>903</v>
+      </c>
+      <c r="W28">
+        <v>8224</v>
+      </c>
+      <c r="X28">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>12995</v>
+      </c>
+      <c r="C29">
+        <v>30807</v>
+      </c>
+      <c r="D29">
+        <v>33184</v>
+      </c>
+      <c r="E29">
+        <v>18246</v>
+      </c>
+      <c r="F29">
+        <v>14611</v>
+      </c>
+      <c r="G29">
+        <v>2946</v>
+      </c>
+      <c r="H29">
+        <v>2906</v>
+      </c>
+      <c r="I29">
+        <v>3510</v>
+      </c>
+      <c r="J29">
+        <v>2942</v>
+      </c>
+      <c r="K29">
+        <v>3637</v>
+      </c>
+      <c r="L29">
+        <v>24233</v>
+      </c>
+      <c r="M29">
+        <v>1776</v>
+      </c>
+      <c r="N29">
+        <v>5788</v>
+      </c>
+      <c r="O29">
+        <v>9129</v>
+      </c>
+      <c r="P29">
+        <v>10039</v>
+      </c>
+      <c r="Q29">
+        <v>6452</v>
+      </c>
+      <c r="R29">
+        <v>2012</v>
+      </c>
+      <c r="S29">
+        <v>2281</v>
+      </c>
+      <c r="T29">
+        <v>5799</v>
+      </c>
+      <c r="U29">
+        <v>4347</v>
+      </c>
+      <c r="V29">
+        <v>4079</v>
+      </c>
+      <c r="W29">
+        <v>5715</v>
+      </c>
+      <c r="X29">
+        <v>2377</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>60929</v>
+      </c>
+      <c r="C30">
+        <v>154839</v>
+      </c>
+      <c r="D30">
+        <v>159622</v>
+      </c>
+      <c r="E30">
+        <v>82826</v>
+      </c>
+      <c r="F30">
+        <v>51713</v>
+      </c>
+      <c r="G30">
+        <v>17733</v>
+      </c>
+      <c r="H30">
+        <v>15114</v>
+      </c>
+      <c r="I30">
+        <v>17668</v>
+      </c>
+      <c r="J30">
+        <v>15672</v>
+      </c>
+      <c r="K30">
+        <v>12475</v>
+      </c>
+      <c r="L30">
+        <v>64562</v>
+      </c>
+      <c r="M30">
+        <v>10019</v>
+      </c>
+      <c r="N30">
+        <v>31242</v>
+      </c>
+      <c r="O30">
+        <v>53649</v>
+      </c>
+      <c r="P30">
+        <v>42304</v>
+      </c>
+      <c r="Q30">
+        <v>22408</v>
+      </c>
+      <c r="R30">
+        <v>7843</v>
+      </c>
+      <c r="S30">
+        <v>12192</v>
+      </c>
+      <c r="T30">
+        <v>18409</v>
+      </c>
+      <c r="U30">
+        <v>12868</v>
+      </c>
+      <c r="V30">
+        <v>2222</v>
+      </c>
+      <c r="W30">
+        <v>11028</v>
+      </c>
+      <c r="X30">
+        <v>4783</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>83697</v>
+      </c>
+      <c r="C31">
+        <v>217948</v>
+      </c>
+      <c r="D31">
+        <v>221278</v>
+      </c>
+      <c r="E31">
+        <v>107416</v>
+      </c>
+      <c r="F31">
+        <v>70258</v>
+      </c>
+      <c r="G31">
+        <v>26080</v>
+      </c>
+      <c r="H31">
+        <v>22887</v>
+      </c>
+      <c r="I31">
+        <v>25288</v>
+      </c>
+      <c r="J31">
+        <v>19948</v>
+      </c>
+      <c r="K31">
+        <v>15574</v>
+      </c>
+      <c r="L31">
+        <v>101521</v>
+      </c>
+      <c r="M31">
+        <v>14320</v>
+      </c>
+      <c r="N31">
+        <v>42164</v>
+      </c>
+      <c r="O31">
+        <v>72397</v>
+      </c>
+      <c r="P31">
+        <v>58083</v>
+      </c>
+      <c r="Q31">
+        <v>34314</v>
+      </c>
+      <c r="R31">
+        <v>11355</v>
+      </c>
+      <c r="S31">
+        <v>17496</v>
+      </c>
+      <c r="T31">
+        <v>32211</v>
+      </c>
+      <c r="U31">
+        <v>22964</v>
+      </c>
+      <c r="V31">
+        <v>1654</v>
+      </c>
+      <c r="W31">
+        <v>15841</v>
+      </c>
+      <c r="X31">
+        <v>3330</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>29027</v>
+      </c>
+      <c r="C32">
+        <v>73598</v>
+      </c>
+      <c r="D32">
+        <v>74493</v>
+      </c>
+      <c r="E32">
+        <v>34010</v>
+      </c>
+      <c r="F32">
+        <v>34120</v>
+      </c>
+      <c r="G32">
+        <v>6084</v>
+      </c>
+      <c r="H32">
+        <v>8139</v>
+      </c>
+      <c r="I32">
+        <v>8372</v>
+      </c>
+      <c r="J32">
+        <v>6840</v>
+      </c>
+      <c r="K32">
+        <v>5676</v>
+      </c>
+      <c r="L32">
+        <v>28698</v>
+      </c>
+      <c r="M32">
+        <v>4520</v>
+      </c>
+      <c r="N32">
+        <v>14735</v>
+      </c>
+      <c r="O32">
+        <v>22535</v>
+      </c>
+      <c r="P32">
+        <v>21616</v>
+      </c>
+      <c r="Q32">
+        <v>11087</v>
+      </c>
+      <c r="R32">
+        <v>3112</v>
+      </c>
+      <c r="S32">
+        <v>3443</v>
+      </c>
+      <c r="T32">
+        <v>7619</v>
+      </c>
+      <c r="U32">
+        <v>6701</v>
+      </c>
+      <c r="V32">
+        <v>2714</v>
+      </c>
+      <c r="W32">
+        <v>5109</v>
+      </c>
+      <c r="X32">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>22548</v>
+      </c>
+      <c r="C33">
+        <v>57170</v>
+      </c>
+      <c r="D33">
+        <v>57800</v>
+      </c>
+      <c r="E33">
+        <v>18837</v>
+      </c>
+      <c r="F33">
+        <v>17638</v>
+      </c>
+      <c r="G33">
+        <v>6583</v>
+      </c>
+      <c r="H33">
+        <v>4807</v>
+      </c>
+      <c r="I33">
+        <v>6013</v>
+      </c>
+      <c r="J33">
+        <v>5412</v>
+      </c>
+      <c r="K33">
+        <v>6316</v>
+      </c>
+      <c r="L33">
+        <v>24618</v>
+      </c>
+      <c r="M33">
+        <v>2837</v>
+      </c>
+      <c r="N33">
+        <v>10849</v>
+      </c>
+      <c r="O33">
+        <v>15560</v>
+      </c>
+      <c r="P33">
+        <v>17280</v>
+      </c>
+      <c r="Q33">
+        <v>11274</v>
+      </c>
+      <c r="R33">
+        <v>2964</v>
+      </c>
+      <c r="S33">
+        <v>9532</v>
+      </c>
+      <c r="T33">
+        <v>6256</v>
+      </c>
+      <c r="U33">
+        <v>4518</v>
+      </c>
+      <c r="V33">
+        <v>85</v>
+      </c>
+      <c r="W33">
+        <v>1263</v>
+      </c>
+      <c r="X33">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>41874</v>
+      </c>
+      <c r="C34">
+        <v>101634</v>
+      </c>
+      <c r="D34">
+        <v>104061</v>
+      </c>
+      <c r="E34">
+        <v>45463</v>
+      </c>
+      <c r="F34">
+        <v>31304</v>
+      </c>
+      <c r="G34">
+        <v>14631</v>
+      </c>
+      <c r="H34">
+        <v>9641</v>
+      </c>
+      <c r="I34">
+        <v>10832</v>
+      </c>
+      <c r="J34">
+        <v>9466</v>
+      </c>
+      <c r="K34">
+        <v>11935</v>
+      </c>
+      <c r="L34">
+        <v>52888</v>
+      </c>
+      <c r="M34">
+        <v>4866</v>
+      </c>
+      <c r="N34">
+        <v>17609</v>
+      </c>
+      <c r="O34">
+        <v>29308</v>
+      </c>
+      <c r="P34">
+        <v>31410</v>
+      </c>
+      <c r="Q34">
+        <v>20868</v>
+      </c>
+      <c r="R34">
+        <v>5943</v>
+      </c>
+      <c r="S34">
+        <v>12165</v>
+      </c>
+      <c r="T34">
+        <v>17554</v>
+      </c>
+      <c r="U34">
+        <v>13290</v>
+      </c>
+      <c r="V34">
+        <v>425</v>
+      </c>
+      <c r="W34">
+        <v>3511</v>
+      </c>
+      <c r="X34">
+        <v>2427</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>39467</v>
+      </c>
+      <c r="C35">
+        <v>87532</v>
+      </c>
+      <c r="D35">
+        <v>88375</v>
+      </c>
+      <c r="E35">
+        <v>47277</v>
+      </c>
+      <c r="F35">
+        <v>27822</v>
+      </c>
+      <c r="G35">
+        <v>14254</v>
+      </c>
+      <c r="H35">
+        <v>6634</v>
+      </c>
+      <c r="I35">
+        <v>8378</v>
+      </c>
+      <c r="J35">
+        <v>7814</v>
+      </c>
+      <c r="K35">
+        <v>16641</v>
+      </c>
+      <c r="L35">
+        <v>38432</v>
+      </c>
+      <c r="M35">
+        <v>3881</v>
+      </c>
+      <c r="N35">
+        <v>13050</v>
+      </c>
+      <c r="O35">
+        <v>21924</v>
+      </c>
+      <c r="P35">
+        <v>30941</v>
+      </c>
+      <c r="Q35">
+        <v>18579</v>
+      </c>
+      <c r="R35">
+        <v>5262</v>
+      </c>
+      <c r="S35">
+        <v>9183</v>
+      </c>
+      <c r="T35">
+        <v>15468</v>
+      </c>
+      <c r="U35">
+        <v>6515</v>
+      </c>
+      <c r="V35">
+        <v>179</v>
+      </c>
+      <c r="W35">
+        <v>1825</v>
+      </c>
+      <c r="X35">
+        <v>843</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>